<commit_message>
mif example and mif template converged
</commit_message>
<xml_diff>
--- a/template_examples/mif_template.xlsx
+++ b/template_examples/mif_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94C76D5-2CC5-9C48-9F50-02E5A4F35B3C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51F3A12-6C5F-A14D-A04C-116989D7E4B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5360" yWindow="3480" windowWidth="23440" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6500" yWindow="6900" windowWidth="22080" windowHeight="10220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mIF" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -62,33 +62,7 @@
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Participant identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-1234.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -101,12 +75,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -119,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="83">
   <si>
     <t>#t</t>
   </si>
@@ -130,21 +104,12 @@
     <t>#p</t>
   </si>
   <si>
-    <t>LEAD ORGANIZATION STUDY ID</t>
-  </si>
-  <si>
     <t>ASSAY CREATOR</t>
   </si>
   <si>
     <t>SLIDE SCANNER MODEL</t>
   </si>
   <si>
-    <t>STAINING PLATFORM</t>
-  </si>
-  <si>
-    <t>AUTOSTAINER MODEL</t>
-  </si>
-  <si>
     <t>IMAGE ANALYSIS SOFTWARE</t>
   </si>
   <si>
@@ -157,9 +122,6 @@
     <t>POSITIVE CELL DETECTION MODEL</t>
   </si>
   <si>
-    <t>PROTOCOL NAME</t>
-  </si>
-  <si>
     <t>Samples</t>
   </si>
   <si>
@@ -208,18 +170,9 @@
     <t>AMPLIFICATION TIME</t>
   </si>
   <si>
-    <t>CIMAC SAMPLE ID</t>
-  </si>
-  <si>
     <t>INTERNAL SLIDE ID</t>
   </si>
   <si>
-    <t>TIME POINT</t>
-  </si>
-  <si>
-    <t>PROTOCOL_NAME</t>
-  </si>
-  <si>
     <t>STAINING DATE</t>
   </si>
   <si>
@@ -241,12 +194,6 @@
     <t>Hamamatsu</t>
   </si>
   <si>
-    <t>auto</t>
-  </si>
-  <si>
-    <t>Leica Bond RX</t>
-  </si>
-  <si>
     <t>InForm</t>
   </si>
   <si>
@@ -256,9 +203,6 @@
     <t>proprietary</t>
   </si>
   <si>
-    <t>T-Cell HSNC</t>
-  </si>
-  <si>
     <t>CD8</t>
   </si>
   <si>
@@ -346,12 +290,6 @@
     <t>07FK 099</t>
   </si>
   <si>
-    <t>PRE</t>
-  </si>
-  <si>
-    <t>T-Cell HNSC</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -364,27 +302,9 @@
     <t>4KHI 021</t>
   </si>
   <si>
-    <t>POST</t>
-  </si>
-  <si>
     <t>8KBI 022</t>
   </si>
   <si>
-    <t>C1D1</t>
-  </si>
-  <si>
-    <t>CIMAC PARTICIPANT ID</t>
-  </si>
-  <si>
-    <t>C036001</t>
-  </si>
-  <si>
-    <t>C036002</t>
-  </si>
-  <si>
-    <t>C036003</t>
-  </si>
-  <si>
     <t>C036001PR.00</t>
   </si>
   <si>
@@ -395,13 +315,40 @@
   </si>
   <si>
     <t>test_prism_trial_id</t>
+  </si>
+  <si>
+    <t>Antibodies</t>
+  </si>
+  <si>
+    <t>Protocol Identifier</t>
+  </si>
+  <si>
+    <t>Staining</t>
+  </si>
+  <si>
+    <t>Bond RX</t>
+  </si>
+  <si>
+    <t>Collection event</t>
+  </si>
+  <si>
+    <t>CIMAC ID</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>Restaging</t>
+  </si>
+  <si>
+    <t>Off_study</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -438,12 +385,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -475,7 +416,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -509,11 +450,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -545,9 +523,17 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -887,15 +873,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N214"/>
+  <dimension ref="A1:N212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -903,31 +889,31 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
     </row>
     <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -946,10 +932,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -968,10 +954,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -990,10 +976,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1012,10 +998,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1029,15 +1015,15 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1051,15 +1037,15 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1078,10 +1064,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1095,147 +1081,191 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B11" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="4">
+        <v>3983272</v>
+      </c>
+      <c r="G13" s="3">
         <v>2</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="H13" s="3">
+        <v>520</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L13" s="6">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="M13" s="6">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="N13" s="6">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="D14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B13" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>28</v>
+      <c r="E14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="4">
+        <v>29387234</v>
+      </c>
+      <c r="G14" s="3">
+        <v>3</v>
+      </c>
+      <c r="H14" s="3">
+        <v>540</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L14" s="6">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="M14" s="6">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="N14" s="6">
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>46</v>
+        <v>11</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="4">
+        <v>2881947</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3">
+        <v>570</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="4">
-        <v>3983272</v>
-      </c>
-      <c r="G15" s="3">
-        <v>2</v>
-      </c>
-      <c r="H15" s="3">
-        <v>520</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="L15" s="6">
-        <v>6.9444444444444441E-3</v>
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="M15" s="6">
         <v>2.7777777777777776E-2</v>
@@ -1246,40 +1276,40 @@
     </row>
     <row r="16" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>53</v>
+        <v>11</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>56</v>
       </c>
       <c r="F16" s="4">
-        <v>29387234</v>
+        <v>293872</v>
       </c>
       <c r="G16" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H16" s="3">
-        <v>540</v>
+        <v>620</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>57</v>
       </c>
       <c r="J16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K16" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="K16" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="L16" s="6">
-        <v>7.6388888888888886E-3</v>
+        <v>9.0277777777777787E-3</v>
       </c>
       <c r="M16" s="6">
         <v>2.7777777777777776E-2</v>
@@ -1290,40 +1320,40 @@
     </row>
     <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="4" t="s">
+      <c r="F17" s="4">
+        <v>392835</v>
+      </c>
+      <c r="G17" s="3">
+        <v>5</v>
+      </c>
+      <c r="H17" s="3">
+        <v>690</v>
+      </c>
+      <c r="I17" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="4">
-        <v>2881947</v>
-      </c>
-      <c r="G17" s="3">
-        <v>1</v>
-      </c>
-      <c r="H17" s="3">
-        <v>570</v>
-      </c>
-      <c r="I17" s="5" t="s">
+      <c r="J17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K17" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="J17" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="L17" s="6">
-        <v>8.3333333333333332E-3</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="M17" s="6">
         <v>2.7777777777777776E-2</v>
@@ -1332,1094 +1362,1003 @@
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="4">
-        <v>293872</v>
-      </c>
-      <c r="G18" s="3">
-        <v>4</v>
-      </c>
-      <c r="H18" s="3">
-        <v>620</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="L18" s="6">
-        <v>9.0277777777777787E-3</v>
-      </c>
-      <c r="M18" s="6">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="N18" s="6">
-        <v>1.0416666666666666E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F19" s="4">
-        <v>392835</v>
-      </c>
-      <c r="G19" s="3">
-        <v>5</v>
-      </c>
-      <c r="H19" s="3">
-        <v>690</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="K19" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="L19" s="6">
-        <v>9.7222222222222224E-3</v>
-      </c>
-      <c r="M19" s="6">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="N19" s="6">
-        <v>1.0416666666666666E-2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A213" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A214" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:N1"/>
-    <mergeCell ref="B13:N13"/>
+    <mergeCell ref="B11:N11"/>
   </mergeCells>
-  <dataValidations count="7">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"DFCI,Mount Sinai, Stanford, MD Anderson"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Vectra 2.0,Hamamatsu"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000003000000}">
-      <formula1>"auto,manual"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"InForm,QuPath"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"proprietary,watershed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"proprietary,random forest classifier"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L15:N214" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L13:N212" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
@@ -2431,10 +2370,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K204"/>
+  <dimension ref="A1:I202"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2443,1174 +2382,1132 @@
     <col min="2" max="98" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B3" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="11">
+        <v>35797</v>
+      </c>
+      <c r="F3" s="11">
+        <v>35797</v>
+      </c>
+      <c r="G3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="11">
+        <v>35798</v>
+      </c>
+      <c r="F4" s="11">
+        <v>35798</v>
+      </c>
+      <c r="G4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>88</v>
+        <v>72</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="F5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G5" s="11">
-        <v>35797</v>
-      </c>
-      <c r="H5" s="11">
-        <v>35797</v>
-      </c>
-      <c r="I5" t="s">
-        <v>77</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+      <c r="E5" s="11">
+        <v>35799</v>
+      </c>
+      <c r="F5" s="11">
+        <v>35799</v>
+      </c>
+      <c r="G5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F6" t="s">
-        <v>76</v>
-      </c>
-      <c r="G6" s="11">
-        <v>35798</v>
-      </c>
-      <c r="H6" s="11">
-        <v>35798</v>
-      </c>
-      <c r="I6" t="s">
-        <v>77</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G7" s="11">
-        <v>35799</v>
-      </c>
-      <c r="H7" s="11">
-        <v>35799</v>
-      </c>
-      <c r="I7" t="s">
-        <v>77</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A203" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A204" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B1:I1"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="G5:H204" xr:uid="{00000000-0002-0000-0100-000000000000}">
-      <formula1>AND(ISNUMBER(G5:G204),LEFT(CELL("format",G5:G204),1)="D")</formula1>
+  <dataValidations count="3">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="G6:H202" xr:uid="{388667F3-E74E-8743-96D0-AD42224921E1}">
+      <formula1>AND(ISNUMBER(G6:G205),LEFT(CELL("format",G6:G205),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I204" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I6:I202 G3:G5" xr:uid="{E13B48FB-F35E-0B40-9917-0FE6424F3239}">
       <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="E3:F5" xr:uid="{88C568AA-B2C1-A741-8821-2F7C4F71C5CD}">
+      <formula1>AND(ISNUMBER(G3:G202),LEFT(CELL("format",G3:G202),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix mif_template antibodies related times
</commit_message>
<xml_diff>
--- a/template_examples/mif_template.xlsx
+++ b/template_examples/mif_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A7CF21-F22F-FA40-BDD7-E39C920A8E6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E65F48-E2CA-B345-BB8E-890B751F90E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1340" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -342,7 +342,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -882,7 +882,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -899,6 +899,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2505,8 +2506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2610,14 +2611,14 @@
       <c r="K3" t="s">
         <v>110</v>
       </c>
-      <c r="L3">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="M3">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="N3">
-        <v>1.0416666666666666E-2</v>
+      <c r="L3" s="6">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="M3" s="6">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="N3" s="6">
+        <v>6.9444444444444447E-4</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -2654,14 +2655,14 @@
       <c r="K4" t="s">
         <v>117</v>
       </c>
-      <c r="L4">
-        <v>7.6388888888888886E-3</v>
-      </c>
-      <c r="M4">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="N4">
-        <v>1.0416666666666666E-2</v>
+      <c r="L4" s="6">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="M4" s="6">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="N4" s="6">
+        <v>6.9444444444444447E-4</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -2698,14 +2699,14 @@
       <c r="K5" t="s">
         <v>117</v>
       </c>
-      <c r="L5">
-        <v>8.3333333333333332E-3</v>
-      </c>
-      <c r="M5">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="N5">
-        <v>1.0416666666666666E-2</v>
+      <c r="L5" s="6">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="M5" s="6">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="N5" s="6">
+        <v>6.9444444444444447E-4</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -2742,14 +2743,14 @@
       <c r="K6" t="s">
         <v>126</v>
       </c>
-      <c r="L6">
-        <v>9.0277777777777787E-3</v>
-      </c>
-      <c r="M6">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="N6">
-        <v>1.0416666666666666E-2</v>
+      <c r="L6" s="6">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="M6" s="6">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="N6" s="6">
+        <v>6.9444444444444447E-4</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -2786,14 +2787,14 @@
       <c r="K7" t="s">
         <v>131</v>
       </c>
-      <c r="L7">
-        <v>9.7222222222222224E-3</v>
-      </c>
-      <c r="M7">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="N7">
-        <v>1.0416666666666666E-2</v>
+      <c r="L7" s="6">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="M7" s="6">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="N7" s="6">
+        <v>6.9444444444444447E-4</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -3776,7 +3777,7 @@
     <mergeCell ref="B1:N1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L3:N202" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L9:N202 M8:N8 L3:N7" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
old-style mif prism tests
</commit_message>
<xml_diff>
--- a/template_examples/mif_template.xlsx
+++ b/template_examples/mif_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E65F48-E2CA-B345-BB8E-890B751F90E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE08E9FC-0BED-E346-8623-25E55EA77AFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1340" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mIF" sheetId="1" r:id="rId1"/>
@@ -329,7 +329,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -381,7 +381,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="131">
   <si>
     <t>LEGEND</t>
   </si>
@@ -671,21 +671,9 @@
     <t>CTTTPP111.00</t>
   </si>
   <si>
-    <t>ABC_INFORM_1</t>
-  </si>
-  <si>
     <t>CTTTPP121.00</t>
   </si>
   <si>
-    <t>ABC_INFORM_2</t>
-  </si>
-  <si>
-    <t>CTTTPP122.00</t>
-  </si>
-  <si>
-    <t>ABC_INFORM_3</t>
-  </si>
-  <si>
     <t>test_prism_trial_id</t>
   </si>
   <si>
@@ -777,6 +765,15 @@
   </si>
   <si>
     <t>1:50</t>
+  </si>
+  <si>
+    <t>ABC_INFORM_121_1</t>
+  </si>
+  <si>
+    <t>ABC_INFORM_121_2</t>
+  </si>
+  <si>
+    <t>ABC_INFORM_111_1</t>
   </si>
 </sst>
 </file>
@@ -1240,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D216"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1267,7 +1264,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1311,7 +1308,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1355,7 +1352,7 @@
         <v>25</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1423,7 +1420,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1431,13 +1428,13 @@
         <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1445,13 +1442,13 @@
         <v>93</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2506,8 +2503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7:N7"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2582,16 +2579,16 @@
         <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F3">
         <v>3983272</v>
@@ -2603,13 +2600,13 @@
         <v>520</v>
       </c>
       <c r="I3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L3" s="6">
         <v>6.9444444444444447E-4</v>
@@ -2626,16 +2623,16 @@
         <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F4">
         <v>29387234</v>
@@ -2647,13 +2644,13 @@
         <v>540</v>
       </c>
       <c r="I4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="J4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="K4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="L4" s="6">
         <v>6.9444444444444447E-4</v>
@@ -2670,16 +2667,16 @@
         <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F5">
         <v>2881947</v>
@@ -2691,13 +2688,13 @@
         <v>570</v>
       </c>
       <c r="I5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="J5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="L5" s="6">
         <v>6.9444444444444447E-4</v>
@@ -2714,16 +2711,16 @@
         <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F6">
         <v>293872</v>
@@ -2735,13 +2732,13 @@
         <v>620</v>
       </c>
       <c r="I6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="J6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="L6" s="6">
         <v>6.9444444444444447E-4</v>
@@ -2758,16 +2755,16 @@
         <v>93</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F7">
         <v>392835</v>
@@ -2779,13 +2776,13 @@
         <v>690</v>
       </c>
       <c r="I7" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="J7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L7" s="6">
         <v>6.9444444444444447E-4</v>

</xml_diff>

<commit_message>
mif template - internal slide id removed
</commit_message>
<xml_diff>
--- a/template_examples/mif_template.xlsx
+++ b/template_examples/mif_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF3B6F2-3098-FD47-BD17-7010331279EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AD881C-B662-7D41-BC47-95CC3E143B92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="460" windowWidth="10000" windowHeight="12320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1340" yWindow="460" windowWidth="26740" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mIF" sheetId="1" r:id="rId1"/>
@@ -132,25 +132,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Identification number used for internal imaging slide.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -158,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -171,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -184,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -381,7 +368,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="116">
   <si>
     <t>LEGEND</t>
   </si>
@@ -678,9 +665,6 @@
   </si>
   <si>
     <t>2.4.2</t>
-  </si>
-  <si>
-    <t>something</t>
   </si>
   <si>
     <t>CD8</t>
@@ -852,11 +836,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1196,10 +1180,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D216"/>
+  <dimension ref="A1:D215"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1212,10 +1196,10 @@
       <c r="A1" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="6"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1310,10 +1294,10 @@
         <v>90</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>99</v>
+        <v>27</v>
+      </c>
+      <c r="C10" s="6">
+        <v>36892</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1321,9 +1305,9 @@
         <v>90</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="7">
+        <v>30</v>
+      </c>
+      <c r="C11" s="6">
         <v>36892</v>
       </c>
     </row>
@@ -1332,42 +1316,45 @@
         <v>90</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="7">
-        <v>36892</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>86</v>
       </c>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+    </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>92</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>41</v>
+        <v>93</v>
+      </c>
+      <c r="B16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1375,7 +1362,7 @@
         <v>93</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1392,7 +1379,7 @@
         <v>96</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" t="s">
         <v>115</v>
@@ -1402,15 +1389,6 @@
       <c r="A19" t="s">
         <v>93</v>
       </c>
-      <c r="B19" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>116</v>
-      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -2389,22 +2367,17 @@
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A216" t="s">
         <v>93</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B14:D14"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C11:C12" xr:uid="{00000000-0002-0000-0000-000006000000}">
-      <formula1>AND(ISNUMBER(C11),LEFT(CELL("format",C11),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C10:C11" xr:uid="{00000000-0002-0000-0000-000006000000}">
+      <formula1>AND(ISNUMBER(C10),LEFT(CELL("format",C10),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2412,6 +2385,12 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
+          <x14:formula1>
+            <xm:f>'Data Dictionary'!H2:H3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C12</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'Data Dictionary'!B2:B5</xm:f>
@@ -2448,12 +2427,6 @@
           </x14:formula1>
           <xm:sqref>C9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
-          <x14:formula1>
-            <xm:f>'Data Dictionary'!H2:H3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C13</xm:sqref>
-        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -2475,21 +2448,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2540,16 +2513,16 @@
         <v>93</v>
       </c>
       <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" t="s">
         <v>100</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>101</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>102</v>
-      </c>
-      <c r="E3" t="s">
-        <v>103</v>
       </c>
       <c r="F3">
         <v>3983272</v>
@@ -2561,13 +2534,13 @@
         <v>520</v>
       </c>
       <c r="I3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" t="s">
         <v>104</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>105</v>
-      </c>
-      <c r="K3" t="s">
-        <v>106</v>
       </c>
       <c r="L3" s="5">
         <v>6.9444444444444447E-4</v>
@@ -2584,16 +2557,16 @@
         <v>93</v>
       </c>
       <c r="B4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" t="s">
         <v>107</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>108</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>109</v>
-      </c>
-      <c r="E4" t="s">
-        <v>110</v>
       </c>
       <c r="F4">
         <v>29387234</v>
@@ -2605,13 +2578,13 @@
         <v>540</v>
       </c>
       <c r="I4" t="s">
+        <v>110</v>
+      </c>
+      <c r="J4" t="s">
         <v>111</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>112</v>
-      </c>
-      <c r="K4" t="s">
-        <v>113</v>
       </c>
       <c r="L4" s="5">
         <v>6.9444444444444447E-4</v>

</xml_diff>

<commit_message>
mif: multiple score files and im3 image per ROI
</commit_message>
<xml_diff>
--- a/template_examples/mif_template.xlsx
+++ b/template_examples/mif_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AD881C-B662-7D41-BC47-95CC3E143B92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA293B89-6013-5B4E-B3A9-767DE96656E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="460" windowWidth="26740" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1300" yWindow="460" windowWidth="16780" windowHeight="13340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mIF" sheetId="1" r:id="rId1"/>
@@ -132,12 +132,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -145,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -158,12 +158,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -171,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -181,6 +181,43 @@
             <family val="2"/>
           </rPr>
           <t>Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as C????????.??</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Path to a file on a user's computer.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>In .txt format</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Path to a file on a user's computer.
+In .im3 format</t>
         </r>
       </text>
     </comment>
@@ -368,7 +405,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="122">
   <si>
     <t>LEGEND</t>
   </si>
@@ -445,12 +482,6 @@
     <t>E.g. 'manual'</t>
   </si>
   <si>
-    <t>Internal slide id</t>
-  </si>
-  <si>
-    <t>Identification number used for internal imaging slide.</t>
-  </si>
-  <si>
     <t>Staining date</t>
   </si>
   <si>
@@ -493,7 +524,16 @@
     <t>Roi id</t>
   </si>
   <si>
-    <t>Data files prefix</t>
+    <t>Score data files</t>
+  </si>
+  <si>
+    <t>Path to a file on a user's computer.</t>
+  </si>
+  <si>
+    <t>Inform export prefix</t>
+  </si>
+  <si>
+    <t>Im3 file</t>
   </si>
   <si>
     <t>Legend for tab 'Antibodies'</t>
@@ -544,9 +584,6 @@
     <t>Fluor wavelength</t>
   </si>
   <si>
-    <t>Number</t>
-  </si>
-  <si>
     <t>Wavelength registered for Alexa Fluor processing.</t>
   </si>
   <si>
@@ -655,74 +692,92 @@
     <t>antibodies</t>
   </si>
   <si>
+    <t>test_prism_trial_id</t>
+  </si>
+  <si>
+    <t>2.4.2</t>
+  </si>
+  <si>
     <t>CTTTPP111.00</t>
   </si>
   <si>
     <t>CTTTPP121.00</t>
   </si>
   <si>
-    <t>test_prism_trial_id</t>
-  </si>
-  <si>
-    <t>2.4.2</t>
+    <t>111/1_score_data.txt,111_extra/1_score_data.txt</t>
+  </si>
+  <si>
+    <t>121/1_score_data.txt</t>
+  </si>
+  <si>
+    <t>121/2_score_data.txt</t>
+  </si>
+  <si>
+    <t>111/1_</t>
+  </si>
+  <si>
+    <t>121/1_</t>
+  </si>
+  <si>
+    <t>121/2_</t>
+  </si>
+  <si>
+    <t>111/1.im3</t>
+  </si>
+  <si>
+    <t>121/1.im3</t>
+  </si>
+  <si>
+    <t>121/2.im3</t>
+  </si>
+  <si>
+    <t>1:200</t>
+  </si>
+  <si>
+    <t>VENTANA</t>
+  </si>
+  <si>
+    <t>1:500</t>
+  </si>
+  <si>
+    <t>9A-ABC</t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>9A11</t>
+  </si>
+  <si>
+    <t>PD-L1</t>
+  </si>
+  <si>
+    <t>1:100</t>
+  </si>
+  <si>
+    <t>DV</t>
+  </si>
+  <si>
+    <t>1:5,000</t>
+  </si>
+  <si>
+    <t>C8-ABC</t>
+  </si>
+  <si>
+    <t>DAKO</t>
+  </si>
+  <si>
+    <t>C8/144b</t>
   </si>
   <si>
     <t>CD8</t>
-  </si>
-  <si>
-    <t>C8/144b</t>
-  </si>
-  <si>
-    <t>DAKO</t>
-  </si>
-  <si>
-    <t>C8-ABC</t>
-  </si>
-  <si>
-    <t>1:5,000</t>
-  </si>
-  <si>
-    <t>DV</t>
-  </si>
-  <si>
-    <t>1:100</t>
-  </si>
-  <si>
-    <t>PD-L1</t>
-  </si>
-  <si>
-    <t>9A11</t>
-  </si>
-  <si>
-    <t>CST</t>
-  </si>
-  <si>
-    <t>9A-ABC</t>
-  </si>
-  <si>
-    <t>1:500</t>
-  </si>
-  <si>
-    <t>VENTANA</t>
-  </si>
-  <si>
-    <t>1:200</t>
-  </si>
-  <si>
-    <t>INFORM_folder_pref_111/1_</t>
-  </si>
-  <si>
-    <t>INFORM_folder_pref_121/1_</t>
-  </si>
-  <si>
-    <t>INFORM_folder_pref_121/2_</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -743,6 +798,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -821,7 +883,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -835,13 +897,14 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1180,10 +1243,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D215"/>
+  <dimension ref="A1:F215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B10" sqref="A10:XFD10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1192,16 +1255,16 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -1209,10 +1272,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -1223,7 +1286,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -1234,7 +1297,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -1245,7 +1308,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -1253,10 +1316,10 @@
         <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>90</v>
       </c>
@@ -1267,7 +1330,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -1278,7 +1341,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>90</v>
       </c>
@@ -1289,168 +1352,194 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>90</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="6">
         <v>36892</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>90</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" s="6">
         <v>36892</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>90</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="7" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>92</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F15" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>93</v>
       </c>
       <c r="B16" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D16" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>93</v>
       </c>
       <c r="B17" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="D17" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
-      <c r="D18" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D18" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>93</v>
       </c>
@@ -2373,63 +2462,15 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B14:F14"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C10:C11" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C10:C11" xr:uid="{1F0D11ED-2B77-1648-9CFA-6AC0824CE266}">
       <formula1>AND(ISNUMBER(C10),LEFT(CELL("format",C10),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
-          <x14:formula1>
-            <xm:f>'Data Dictionary'!H2:H3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C12</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
-          <x14:formula1>
-            <xm:f>'Data Dictionary'!B2:B5</xm:f>
-          </x14:formula1>
-          <xm:sqref>C3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
-          <x14:formula1>
-            <xm:f>'Data Dictionary'!C2:C3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
-          <x14:formula1>
-            <xm:f>'Data Dictionary'!D2:D3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
-          <x14:formula1>
-            <xm:f>'Data Dictionary'!E2:E3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
-          <x14:formula1>
-            <xm:f>'Data Dictionary'!F2:F3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C8</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
-          <x14:formula1>
-            <xm:f>'Data Dictionary'!G2:G3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C9</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2437,8 +2478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N202"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:L4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:N202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2447,47 +2488,47 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>92</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>60</v>
@@ -2513,16 +2554,16 @@
         <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="F3">
         <v>3983272</v>
@@ -2534,21 +2575,21 @@
         <v>520</v>
       </c>
       <c r="I3" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="J3" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="K3" t="s">
-        <v>105</v>
-      </c>
-      <c r="L3" s="5">
+        <v>115</v>
+      </c>
+      <c r="L3" s="8">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="8">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="8">
         <v>6.9444444444444447E-4</v>
       </c>
     </row>
@@ -2557,16 +2598,16 @@
         <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D4" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F4">
         <v>29387234</v>
@@ -2581,18 +2622,18 @@
         <v>110</v>
       </c>
       <c r="J4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K4" t="s">
-        <v>112</v>
-      </c>
-      <c r="L4" s="5">
+        <v>108</v>
+      </c>
+      <c r="L4" s="8">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="8">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="8">
         <v>6.9444444444444447E-4</v>
       </c>
     </row>
@@ -2600,25 +2641,25 @@
       <c r="A5" t="s">
         <v>93</v>
       </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>93</v>
       </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>93</v>
       </c>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -3612,7 +3653,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:E33"/>
+  <dimension ref="B1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3742,18 +3783,18 @@
         <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
         <v>29</v>
@@ -3764,51 +3805,51 @@
         <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
         <v>31</v>
       </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" spans="2:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E14" t="s">
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
+      <c r="C15" t="s">
         <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
@@ -3819,156 +3860,167 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="3" t="s">
+    <row r="21" spans="2:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
         <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
         <v>54</v>
-      </c>
-      <c r="C26" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" t="s">
         <v>57</v>
-      </c>
-      <c r="C27" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
         <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
         <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
         <v>67</v>
       </c>
       <c r="D32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s">
         <v>67</v>
       </c>
       <c r="D33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" t="s">
         <v>72</v>
       </c>
     </row>
@@ -4009,7 +4061,7 @@
         <v>22</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
mif assay feedback impl: added panel and antibodies export names
</commit_message>
<xml_diff>
--- a/template_examples/mif_template.xlsx
+++ b/template_examples/mif_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA293B89-6013-5B4E-B3A9-767DE96656E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA28F3C-C059-F341-9EB6-F62119FE4ED0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="460" windowWidth="16780" windowHeight="13340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1280" yWindow="460" windowWidth="20000" windowHeight="15220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mIF" sheetId="1" r:id="rId1"/>
@@ -171,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -184,30 +184,47 @@
         </r>
       </text>
     </comment>
-    <comment ref="D15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Path to a file on a user's computer.
-</t>
+          <t>Identifier of a region of interest within one mIF slide, e.g. 1, 2, 3 or [123 x 321]</t>
         </r>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+      <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>In .txt format</t>
+          <t>A comma-separated list of paths to files on a user's computer.
+In .txt format</t>
         </r>
       </text>
     </comment>
-    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="E16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Path on a user's computer to an InForm export directory with ROI's export prefix</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -236,7 +253,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -253,7 +270,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Resulting type of antibody clone from primary antibody sample.</t>
+          <t>Name of this antibody in InForm export, e.g. 'CD8 (Opal 520)'</t>
         </r>
       </text>
     </comment>
@@ -266,7 +283,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Company from which antibody sample was derived.</t>
+          <t>Resulting type of antibody clone from primary antibody sample.</t>
         </r>
       </text>
     </comment>
@@ -279,7 +296,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Antibody registry catalog number assigned to antibody sample.</t>
+          <t>Company from which antibody sample was derived.</t>
         </r>
       </text>
     </comment>
@@ -292,7 +309,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Identification number assigned to the particular quantity or lot of material from manufacturer.</t>
+          <t>Antibody registry catalog number assigned to antibody sample.</t>
         </r>
       </text>
     </comment>
@@ -305,7 +322,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Order of staining applied</t>
+          <t>Identification number assigned to the particular quantity or lot of material from manufacturer.</t>
         </r>
       </text>
     </comment>
@@ -318,7 +335,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Wavelength registered for Alexa Fluor processing.</t>
+          <t>Order of staining applied</t>
         </r>
       </text>
     </comment>
@@ -331,7 +348,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Concentration ratio for primary antibody dilution.</t>
+          <t>Wavelength registered for Alexa Fluor processing.</t>
         </r>
       </text>
     </comment>
@@ -344,7 +361,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Dilution agent used for antibody sample.</t>
+          <t>Concentration ratio for primary antibody dilution.</t>
         </r>
       </text>
     </comment>
@@ -353,11 +370,11 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Concentration ratio for fluor dilution agent.</t>
+          <t>Dilution agent used for antibody sample.</t>
         </r>
       </text>
     </comment>
@@ -366,11 +383,11 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Length of time needed for antigen retrieval.</t>
+          <t>Concentration ratio for fluor dilution agent.</t>
         </r>
       </text>
     </comment>
@@ -383,11 +400,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Length of time needed for antigen retrieval.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Length of time for primary antibody incubation.</t>
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
+    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -405,7 +435,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="135">
   <si>
     <t>LEGEND</t>
   </si>
@@ -506,6 +536,12 @@
     <t>E.g. 'Yes'</t>
   </si>
   <si>
+    <t>Panel</t>
+  </si>
+  <si>
+    <t>E.g. 'Panel 1: PD-L1, CD68, PD-1, CD8, CD3, pan-cytokeratin, DAPI'</t>
+  </si>
+  <si>
     <t>Section 'ROIs' of tab 'mIF'</t>
   </si>
   <si>
@@ -524,18 +560,27 @@
     <t>Roi id</t>
   </si>
   <si>
+    <t>Identifier of a region of interest within one mIF slide, e.g. 1, 2, 3 or [123 x 321]</t>
+  </si>
+  <si>
     <t>Score data files</t>
   </si>
   <si>
+    <t>A comma-separated list of paths to files on a user's computer.</t>
+  </si>
+  <si>
+    <t>Inform export prefix</t>
+  </si>
+  <si>
+    <t>Path on a user's computer to an InForm export directory with ROI's export prefix</t>
+  </si>
+  <si>
+    <t>Im3 file</t>
+  </si>
+  <si>
     <t>Path to a file on a user's computer.</t>
   </si>
   <si>
-    <t>Inform export prefix</t>
-  </si>
-  <si>
-    <t>Im3 file</t>
-  </si>
-  <si>
     <t>Legend for tab 'Antibodies'</t>
   </si>
   <si>
@@ -548,6 +593,12 @@
     <t>Antibody type collected for this study.</t>
   </si>
   <si>
+    <t>Export name</t>
+  </si>
+  <si>
+    <t>Name of this antibody in InForm export, e.g. 'CD8 (Opal 520)'</t>
+  </si>
+  <si>
     <t>Clone</t>
   </si>
   <si>
@@ -671,6 +722,18 @@
     <t>No</t>
   </si>
   <si>
+    <t>Panel 1: PD-L1, CD68, PD-1, CD8, CD3, pan-cytokeratin, DAPI</t>
+  </si>
+  <si>
+    <t>Panel 2: FOXP3, Granzyme B, CD45RO, CD8, CD3, pan-cytokeratin, DAPI</t>
+  </si>
+  <si>
+    <t>Panel 3: pan-cytokeratin, CD8, PD-1, PD-L1, DAPI</t>
+  </si>
+  <si>
+    <t>Panel 4: SOX10, CD8, PD-1, PD-L1, DAPI</t>
+  </si>
+  <si>
     <t>#t</t>
   </si>
   <si>
@@ -701,76 +764,82 @@
     <t>CTTTPP111.00</t>
   </si>
   <si>
+    <t>111/1_score_data.txt,111_extra/1_score_data.txt</t>
+  </si>
+  <si>
+    <t>111/1_</t>
+  </si>
+  <si>
+    <t>111/1.im3</t>
+  </si>
+  <si>
     <t>CTTTPP121.00</t>
   </si>
   <si>
-    <t>111/1_score_data.txt,111_extra/1_score_data.txt</t>
-  </si>
-  <si>
     <t>121/1_score_data.txt</t>
   </si>
   <si>
+    <t>121/1_</t>
+  </si>
+  <si>
+    <t>121/1.im3</t>
+  </si>
+  <si>
     <t>121/2_score_data.txt</t>
   </si>
   <si>
-    <t>111/1_</t>
-  </si>
-  <si>
-    <t>121/1_</t>
-  </si>
-  <si>
     <t>121/2_</t>
   </si>
   <si>
-    <t>111/1.im3</t>
-  </si>
-  <si>
-    <t>121/1.im3</t>
-  </si>
-  <si>
     <t>121/2.im3</t>
   </si>
   <si>
+    <t>CD8</t>
+  </si>
+  <si>
+    <t>C8/144b</t>
+  </si>
+  <si>
+    <t>DAKO</t>
+  </si>
+  <si>
+    <t>C8-ABC</t>
+  </si>
+  <si>
+    <t>1:5,000</t>
+  </si>
+  <si>
+    <t>DV</t>
+  </si>
+  <si>
+    <t>1:100</t>
+  </si>
+  <si>
+    <t>PD-L1</t>
+  </si>
+  <si>
+    <t>9A11</t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>9A-ABC</t>
+  </si>
+  <si>
+    <t>1:500</t>
+  </si>
+  <si>
+    <t>VENTANA</t>
+  </si>
+  <si>
     <t>1:200</t>
   </si>
   <si>
-    <t>VENTANA</t>
-  </si>
-  <si>
-    <t>1:500</t>
-  </si>
-  <si>
-    <t>9A-ABC</t>
-  </si>
-  <si>
-    <t>CST</t>
-  </si>
-  <si>
-    <t>9A11</t>
-  </si>
-  <si>
-    <t>PD-L1</t>
-  </si>
-  <si>
-    <t>1:100</t>
-  </si>
-  <si>
-    <t>DV</t>
-  </si>
-  <si>
-    <t>1:5,000</t>
-  </si>
-  <si>
-    <t>C8-ABC</t>
-  </si>
-  <si>
-    <t>DAKO</t>
-  </si>
-  <si>
-    <t>C8/144b</t>
-  </si>
-  <si>
-    <t>CD8</t>
+    <t>CD8 (Opal 540)</t>
+  </si>
+  <si>
+    <t>PD-L1 (Opal 620)</t>
   </si>
 </sst>
 </file>
@@ -809,7 +878,7 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Tahoma"/>
+      <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -883,7 +952,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -897,14 +966,15 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1243,10 +1313,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F215"/>
+  <dimension ref="A1:F216"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1257,1229 +1327,1252 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C1" s="5"/>
+        <v>99</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>36892</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>36892</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>92</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="B15" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" t="s">
-        <v>97</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" t="s">
-        <v>102</v>
-      </c>
-      <c r="F16" t="s">
-        <v>105</v>
+        <v>103</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B17" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>100</v>
+      <c r="D17" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="E17" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="F17" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>101</v>
+        <v>1</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="E18" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="F18" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>104</v>
+      </c>
+      <c r="B19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>93</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C10:C11" xr:uid="{1F0D11ED-2B77-1648-9CFA-6AC0824CE266}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C10:C11" xr:uid="{E515833F-31D5-DC48-8F40-EEC834994C0B}">
       <formula1>AND(ISNUMBER(C10),LEFT(CELL("format",C10),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000009000000}">
+          <x14:formula1>
+            <xm:f>'Data Dictionary'!$I$2:$I$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C13</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N202"/>
+  <dimension ref="A1:O202"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:N202"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2488,1160 +2581,1161 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B1" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" t="s">
         <v>121</v>
       </c>
-      <c r="C3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G3">
         <v>3983272</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>2</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>520</v>
       </c>
-      <c r="I3" t="s">
-        <v>117</v>
-      </c>
       <c r="J3" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="K3" t="s">
-        <v>115</v>
-      </c>
-      <c r="L3" s="8">
+        <v>124</v>
+      </c>
+      <c r="L3" t="s">
+        <v>125</v>
+      </c>
+      <c r="M3" s="7">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="M3" s="8">
+      <c r="N3" s="7">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="N3" s="8">
+      <c r="O3" s="7">
         <v>6.9444444444444447E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C4" t="s">
-        <v>113</v>
+        <v>126</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>134</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F4">
+        <v>128</v>
+      </c>
+      <c r="F4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4">
         <v>29387234</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>3</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>540</v>
       </c>
-      <c r="I4" t="s">
-        <v>110</v>
-      </c>
       <c r="J4" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="K4" t="s">
-        <v>108</v>
-      </c>
-      <c r="L4" s="8">
+        <v>131</v>
+      </c>
+      <c r="L4" t="s">
+        <v>132</v>
+      </c>
+      <c r="M4" s="7">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="M4" s="8">
+      <c r="N4" s="7">
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="N4" s="8">
+      <c r="O4" s="7">
         <v>6.9444444444444447E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>93</v>
-      </c>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>93</v>
-      </c>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>93</v>
-      </c>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:N1"/>
+    <mergeCell ref="B1:O1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L9:N202 M8:N8 L3:N7" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="M5:O202 M3:O4" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
@@ -3653,7 +3747,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:E34"/>
+  <dimension ref="B1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3815,213 +3909,241 @@
       </c>
     </row>
     <row r="14" spans="2:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
         <v>34</v>
       </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="15" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="D15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
         <v>38</v>
       </c>
-      <c r="C16" t="s">
-        <v>3</v>
+      <c r="E16" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
       </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="32" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
         <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="D30" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C31" t="s">
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C32" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C34" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D34" t="s">
-        <v>72</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B35" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B36" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -4032,7 +4154,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:H5"/>
+  <dimension ref="B1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4041,7 +4163,7 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
@@ -4063,61 +4185,76 @@
       <c r="H1" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="E2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>81</v>
       </c>
-      <c r="F2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>74</v>
-      </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>82</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
         <v>83</v>
       </c>
-      <c r="G3" t="s">
-        <v>85</v>
-      </c>
-      <c r="H3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>76</v>
+      <c r="I5" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CIDC-1127 add report to mif_assay schema
</commit_message>
<xml_diff>
--- a/template_examples/mif_template.xlsx
+++ b/template_examples/mif_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/VSCodeProjects/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4281C4-514F-4C44-B1B5-FC7F33EA3CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068EFC0A-EC8D-474B-9BC3-FD950E9E441B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="1760" windowWidth="23260" windowHeight="12580" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2080" yWindow="1760" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mIF" sheetId="1" r:id="rId1"/>
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8280" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8281" uniqueCount="156">
   <si>
     <t>LEGEND</t>
   </si>
@@ -1028,6 +1028,9 @@
   </si>
   <si>
     <t>Failed QC</t>
+  </si>
+  <si>
+    <t>qc_report.zip</t>
   </si>
 </sst>
 </file>
@@ -1532,8 +1535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2017"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1689,7 +1692,9 @@
       <c r="B14" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C14" s="9"/>
+      <c r="C14" s="9" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -32579,7 +32584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A5F282A-3E87-AC4E-97AF-DDCC4881B63B}">
   <dimension ref="A1:C2002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>